<commit_message>
drt tables, comment fields
</commit_message>
<xml_diff>
--- a/static/documents/drt/en/c20.xlsx
+++ b/static/documents/drt/en/c20.xlsx
@@ -18,41 +18,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
-    <t>a fertőzés típusa:</t>
-  </si>
-  <si>
-    <t>3.  Principal diagnosis code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.  Is patient allergic to aspirin? </t>
-  </si>
-  <si>
     <t>(yes = 1;
 no = 0)</t>
   </si>
   <si>
-    <t>6.  Is there a known contraindication or intolerance of aspirin?</t>
-  </si>
-  <si>
-    <t>7.  Type of discharge:</t>
-  </si>
-  <si>
     <t>If other, specify</t>
-  </si>
-  <si>
-    <t>8. Is there a known objection/refusal to take aspirin-containing medication?</t>
-  </si>
-  <si>
-    <t>9.   Was patient prescribed at discharge to take aspirin?</t>
   </si>
   <si>
     <t>(yes= 1;
 no = 0)</t>
   </si>
   <si>
-    <t>11. Date of discharge</t>
-  </si>
-  <si>
     <t>(YYYY-MM-DD)
 (1970-01-31)</t>
   </si>
@@ -67,40 +43,64 @@
     <t>AMI patients prescribed aspirin at discharge</t>
   </si>
   <si>
-    <t>10. Was patient prescribed to take other (non-aspirin-containing) platelet aggregation inhibitor therapy?</t>
-  </si>
-  <si>
     <t xml:space="preserve">The data in the light blue area should be used for the upload into the IT platform. </t>
-  </si>
-  <si>
-    <t>etc</t>
-  </si>
-  <si>
-    <t>1. Patient ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Date of birth </t>
-  </si>
-  <si>
-    <t>4. Type of unit</t>
   </si>
   <si>
     <t>1. acute
 2. rehab.</t>
   </si>
   <si>
-    <t>1 = transfer to another inpatient hospital 
-2 = discharge to home, social home
-3 = patient left hospital against medical advice 
-4= in hospital death
-5 = other</t>
+    <t>0 = transfer to another inpatient hospital 
+1 = discharge to home, social home
+2 = patient left hospital against medical advice 
+3= in hospital death
+4= other</t>
+  </si>
+  <si>
+    <t>1. Case ID</t>
+  </si>
+  <si>
+    <t>2. Hospital registration number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Date of birth </t>
+  </si>
+  <si>
+    <t>4.  Principal diagnosis code</t>
+  </si>
+  <si>
+    <t>5. Type of unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.  Is patient allergic to aspirin? </t>
+  </si>
+  <si>
+    <t>7.  Is there a known contraindication or intolerance of aspirin?</t>
+  </si>
+  <si>
+    <t>8.  Type of discharge:</t>
+  </si>
+  <si>
+    <t>9. Is there a known objection/refusal to take aspirin-containing medication?</t>
+  </si>
+  <si>
+    <t>10.   Was patient prescribed at discharge to take aspirin?</t>
+  </si>
+  <si>
+    <t>11. Was patient prescribed to take other (non-aspirin-containing) platelet aggregation inhibitor therapy?</t>
+  </si>
+  <si>
+    <t>12. Date of discharge</t>
+  </si>
+  <si>
+    <t>13. Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,13 +127,6 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -169,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -178,10 +171,158 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -191,32 +332,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -230,10 +349,47 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -242,48 +398,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,151 +759,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="14" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="20.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="20.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="5" spans="1:15" ht="15" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="F5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="7.5" customHeight="1" thickBot="1"/>
-    <row r="5" spans="1:13" ht="15" customHeight="1">
-      <c r="B5" s="11" t="s">
+      <c r="H5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="K5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="L5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="111" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="11" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="23"/>
+    </row>
+    <row r="7" spans="1:15" ht="51.75" thickBot="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="L7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="86.25" customHeight="1">
-      <c r="B6" s="15"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="1:13" ht="111.75" customHeight="1">
-      <c r="B7" s="15"/>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>2</v>
-      </c>
+      <c r="N7" s="25"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -737,11 +922,10 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10">
-        <v>3</v>
-      </c>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -754,11 +938,10 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11">
-        <v>4</v>
-      </c>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -771,11 +954,10 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12">
-        <v>5</v>
-      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -788,11 +970,10 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13">
-        <v>6</v>
-      </c>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -805,11 +986,10 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14">
-        <v>7</v>
-      </c>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -822,11 +1002,10 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15">
-        <v>8</v>
-      </c>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -839,11 +1018,10 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16">
-        <v>9</v>
-      </c>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -856,11 +1034,10 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17">
-        <v>10</v>
-      </c>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -873,11 +1050,10 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18">
-        <v>11</v>
-      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -890,11 +1066,10 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19">
-        <v>12</v>
-      </c>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -907,11 +1082,10 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20">
-        <v>13</v>
-      </c>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -924,11 +1098,10 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21">
-        <v>14</v>
-      </c>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -941,11 +1114,10 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22">
-        <v>15</v>
-      </c>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -958,11 +1130,10 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23">
-        <v>16</v>
-      </c>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -975,11 +1146,10 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24">
-        <v>17</v>
-      </c>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -992,11 +1162,10 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25">
-        <v>18</v>
-      </c>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1009,11 +1178,10 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26">
-        <v>19</v>
-      </c>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1026,11 +1194,10 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27">
-        <v>20</v>
-      </c>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1043,11 +1210,10 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28">
-        <v>21</v>
-      </c>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1060,11 +1226,10 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29">
-        <v>22</v>
-      </c>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1077,11 +1242,10 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30">
-        <v>23</v>
-      </c>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1094,11 +1258,10 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31">
-        <v>24</v>
-      </c>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1111,11 +1274,10 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32">
-        <v>25</v>
-      </c>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1128,11 +1290,10 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33">
-        <v>26</v>
-      </c>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1145,11 +1306,10 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34">
-        <v>27</v>
-      </c>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1162,11 +1322,10 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35">
-        <v>28</v>
-      </c>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1179,11 +1338,10 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36">
-        <v>29</v>
-      </c>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1196,11 +1354,10 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37">
-        <v>30</v>
-      </c>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1213,11 +1370,10 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38">
-        <v>31</v>
-      </c>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1230,11 +1386,10 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39">
-        <v>32</v>
-      </c>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1247,11 +1402,10 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40">
-        <v>33</v>
-      </c>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1264,11 +1418,10 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41">
-        <v>34</v>
-      </c>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1281,11 +1434,10 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42">
-        <v>35</v>
-      </c>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1298,11 +1450,10 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43">
-        <v>36</v>
-      </c>
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1315,11 +1466,10 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44">
-        <v>37</v>
-      </c>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1332,11 +1482,10 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45">
-        <v>38</v>
-      </c>
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1349,11 +1498,10 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46">
-        <v>39</v>
-      </c>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1366,11 +1514,10 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47">
-        <v>40</v>
-      </c>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1383,11 +1530,10 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48">
-        <v>41</v>
-      </c>
+      <c r="N47" s="1"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1400,11 +1546,10 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49">
-        <v>42</v>
-      </c>
+      <c r="N48" s="1"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1417,11 +1562,10 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50">
-        <v>43</v>
-      </c>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1434,11 +1578,10 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51">
-        <v>44</v>
-      </c>
+      <c r="N50" s="1"/>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1451,11 +1594,10 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52">
-        <v>45</v>
-      </c>
+      <c r="N51" s="1"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1468,11 +1610,10 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53">
-        <v>46</v>
-      </c>
+      <c r="N52" s="1"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1485,11 +1626,10 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54">
-        <v>47</v>
-      </c>
+      <c r="N53" s="1"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1502,11 +1642,10 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55">
-        <v>48</v>
-      </c>
+      <c r="N54" s="1"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1519,11 +1658,10 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56">
-        <v>49</v>
-      </c>
+      <c r="N55" s="1"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1536,11 +1674,10 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57">
-        <v>50</v>
-      </c>
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1553,11 +1690,10 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" t="s">
-        <v>17</v>
-      </c>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1570,20 +1706,25 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:J6"/>
+  <mergeCells count="15">
+    <mergeCell ref="N5:N7"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:H7"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>